<commit_message>
Domino Qi Mini Rev. B: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
+++ b/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
@@ -8,26 +8,27 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Qi Mini Rev. A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Qi Mini Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$2:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -811,15 +812,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.88235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5686274509804"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.5960784313726"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0470588235294"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domino Qi Mini Rev. C: changed NTB0102GU to NTB0102GF
</commit_message>
<xml_diff>
--- a/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
+++ b/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
@@ -8,27 +8,29 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Qi Mini Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Qi Mini Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$2:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -655,16 +657,16 @@
     <t>IC TRANSLATING TXRX 12XQFN</t>
   </si>
   <si>
-    <t>NTB0102GU</t>
-  </si>
-  <si>
-    <t>XQFN-10</t>
+    <t>NTB0102GF</t>
+  </si>
+  <si>
+    <t>SOT1089</t>
   </si>
   <si>
     <t>U5</t>
   </si>
   <si>
-    <t>IC TRANSLATING TXRX 10XQFN</t>
+    <t>TXRX TRANSLATING DUAL 3ST 8XSON</t>
   </si>
   <si>
     <t>MAX3375EEKA+T</t>
@@ -783,11 +785,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -808,19 +811,19 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H44" activeCellId="0" pane="topLeft" sqref="H44"/>
+      <selection activeCell="C48" activeCellId="0" pane="topLeft" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2549019607843"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -2041,13 +2044,13 @@
       <c r="E47" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="2" t="s">
         <v>207</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="H47" s="2" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Domino Qi Mini Rev. D: corrected bridge pinout
</commit_message>
<xml_diff>
--- a/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
+++ b/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Qi Mini Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Qi Mini Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$2:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -815,15 +816,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Changed Domino Qi Mini to 4 layers
</commit_message>
<xml_diff>
--- a/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
+++ b/Domino Qi Mini/BOM/Domino Qi Mini BOM.xlsx
@@ -5,33 +5,34 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="114" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Qi Mini Rev. D" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Qi Mini Rev. E" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$2:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Qi Mini Rev. E'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -705,37 +706,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -747,13 +748,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000066CC"/>
-        <bgColor rgb="00008080"/>
+        <fgColor rgb="FF0066CC"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -762,44 +763,51 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -811,22 +819,24 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C48" activeCellId="0" pane="topLeft" sqref="C48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.98469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -881,7 +891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -907,7 +917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -933,7 +943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -959,7 +969,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -985,7 +995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -1167,7 +1177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -1193,7 +1203,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -1219,7 +1229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -1245,7 +1255,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -1323,7 +1333,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -1349,7 +1359,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -1375,7 +1385,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -1401,7 +1411,7 @@
         <v>101</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -1479,7 +1489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
@@ -1505,7 +1515,7 @@
         <v>121</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
@@ -1531,7 +1541,7 @@
         <v>125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
@@ -1557,7 +1567,7 @@
         <v>129</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
@@ -1583,7 +1593,7 @@
         <v>133</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
@@ -1609,7 +1619,7 @@
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
@@ -1661,7 +1671,7 @@
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
@@ -1687,7 +1697,7 @@
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
@@ -1713,7 +1723,7 @@
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -1739,7 +1749,7 @@
         <v>156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>160</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>164</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
@@ -1817,7 +1827,7 @@
         <v>168</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>172</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>176</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
@@ -1895,7 +1905,7 @@
         <v>182</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row r="42" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
@@ -1921,7 +1931,7 @@
         <v>185</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
@@ -1947,7 +1957,7 @@
         <v>190</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row r="44" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
@@ -1976,7 +1986,7 @@
         <v>197</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row r="45" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
@@ -2002,7 +2012,7 @@
         <v>201</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row r="46" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
@@ -2028,7 +2038,7 @@
         <v>205</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
+    <row r="47" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
@@ -2054,7 +2064,7 @@
         <v>209</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row r="48" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
@@ -2080,7 +2090,7 @@
         <v>214</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+    <row r="49" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
@@ -2109,7 +2119,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.38611111111111" bottom="0.886111111111111" header="0.7875" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"FreeSans,Normal"&amp;36&amp;A</oddHeader>
     <oddFooter/>

</xml_diff>